<commit_message>
1/3 excel interfaces done, but have to add backup functionality to download button
</commit_message>
<xml_diff>
--- a/public/formatos/FormatoDataAlmacenes/Formato Data de Silos, Almacenes, Depósitos 2025.xlsx
+++ b/public/formatos/FormatoDataAlmacenes/Formato Data de Silos, Almacenes, Depósitos 2025.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="67">
   <si>
     <t>TIPO DE EVENTO</t>
   </si>
@@ -168,6 +168,54 @@
   </si>
   <si>
     <t>nombre2</t>
+  </si>
+  <si>
+    <t>nosealv</t>
+  </si>
+  <si>
+    <t>03/04/2025</t>
+  </si>
+  <si>
+    <t>19/04/2025</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>11/04/2025</t>
+  </si>
+  <si>
+    <t>adasdasda</t>
+  </si>
+  <si>
+    <t>10/04/2025</t>
+  </si>
+  <si>
+    <t>26/04/2025</t>
+  </si>
+  <si>
+    <t>estado2</t>
+  </si>
+  <si>
+    <t>municipio2</t>
+  </si>
+  <si>
+    <t>parroquia2</t>
+  </si>
+  <si>
+    <t>sector2</t>
+  </si>
+  <si>
+    <t>J-20000002-2</t>
+  </si>
+  <si>
+    <t>Yuca</t>
+  </si>
+  <si>
+    <t>nombre_responsable2</t>
+  </si>
+  <si>
+    <t>02/05/2025</t>
   </si>
 </sst>
 </file>
@@ -1325,62 +1373,170 @@
       </c>
     </row>
     <row r="8" spans="1:67" customHeight="1" ht="33">
-      <c r="A8" s="16"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="62"/>
-      <c r="Q8" s="62"/>
-      <c r="R8" s="70"/>
-      <c r="S8" s="62"/>
-      <c r="T8" s="62"/>
-      <c r="U8" s="62"/>
-      <c r="V8" s="62"/>
-      <c r="W8" s="62"/>
-      <c r="X8" s="63"/>
-      <c r="Y8" s="62"/>
-      <c r="Z8" s="62"/>
-      <c r="AA8" s="62"/>
+      <c r="A8" s="16">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="8">
+        <v>4</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="N8" s="8">
+        <v>5</v>
+      </c>
+      <c r="O8" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="P8" s="62">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="62">
+        <v>2</v>
+      </c>
+      <c r="R8" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="S8" s="62" t="s">
+        <v>45</v>
+      </c>
+      <c r="T8" s="62">
+        <v>10000001</v>
+      </c>
+      <c r="U8" s="62">
+        <v>10000000001</v>
+      </c>
+      <c r="V8" s="62" t="s">
+        <v>46</v>
+      </c>
+      <c r="W8" s="62" t="s">
+        <v>47</v>
+      </c>
+      <c r="X8" s="63" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y8" s="62" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z8" s="62" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA8" s="62">
+        <v>20000000002</v>
+      </c>
     </row>
     <row r="9" spans="1:67" customHeight="1" ht="33">
-      <c r="A9" s="16"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="62"/>
-      <c r="Q9" s="62"/>
-      <c r="R9" s="70"/>
-      <c r="S9" s="62"/>
-      <c r="T9" s="62"/>
-      <c r="U9" s="62"/>
-      <c r="V9" s="62"/>
-      <c r="W9" s="62"/>
-      <c r="X9" s="63"/>
-      <c r="Y9" s="62"/>
-      <c r="Z9" s="62"/>
-      <c r="AA9" s="62"/>
+      <c r="A9" s="16">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="8">
+        <v>3</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="N9" s="8">
+        <v>5</v>
+      </c>
+      <c r="O9" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="P9" s="62">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="62">
+        <v>1</v>
+      </c>
+      <c r="R9" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="S9" s="62" t="s">
+        <v>65</v>
+      </c>
+      <c r="T9" s="62">
+        <v>20000002</v>
+      </c>
+      <c r="U9" s="62">
+        <v>20000000002</v>
+      </c>
+      <c r="V9" s="62" t="s">
+        <v>46</v>
+      </c>
+      <c r="W9" s="62" t="s">
+        <v>47</v>
+      </c>
+      <c r="X9" s="63" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y9" s="62" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z9" s="62" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA9" s="62">
+        <v>20000000002</v>
+      </c>
     </row>
     <row r="10" spans="1:67" customHeight="1" ht="33" s="7" customFormat="1">
       <c r="A10" s="16"/>

</xml_diff>

<commit_message>
Last interface changes, excel exports fixed, maybe add backup module to finish
</commit_message>
<xml_diff>
--- a/public/formatos/FormatoDataAlmacenes/Formato Data de Silos, Almacenes, Depósitos 2025.xlsx
+++ b/public/formatos/FormatoDataAlmacenes/Formato Data de Silos, Almacenes, Depósitos 2025.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
   <si>
     <t>TIPO DE EVENTO</t>
   </si>
@@ -116,106 +116,55 @@
     <t>NUMERO DE TELEFONO DEL TECNICO.</t>
   </si>
   <si>
-    <t>asdasdasd</t>
-  </si>
-  <si>
-    <t>08/03/2025</t>
-  </si>
-  <si>
-    <t>22/03/2025</t>
-  </si>
-  <si>
-    <t>estado1</t>
-  </si>
-  <si>
-    <t>municipio1</t>
-  </si>
-  <si>
-    <t>parroquia1</t>
-  </si>
-  <si>
-    <t>sector1</t>
-  </si>
-  <si>
-    <t>nombre1</t>
-  </si>
-  <si>
-    <t>J-10000001-1</t>
-  </si>
-  <si>
-    <t>Auyama</t>
-  </si>
-  <si>
-    <t>unidades</t>
-  </si>
-  <si>
-    <t>Unaquenoconozco</t>
-  </si>
-  <si>
-    <t>nombre_responsable1</t>
-  </si>
-  <si>
-    <t>Quemalo</t>
+    <t>02/04/2025</t>
+  </si>
+  <si>
+    <t>04/04/2025</t>
+  </si>
+  <si>
+    <t>Monagas</t>
+  </si>
+  <si>
+    <t>Caripe</t>
+  </si>
+  <si>
+    <t>Teresén</t>
+  </si>
+  <si>
+    <t>Los Cigarrones</t>
+  </si>
+  <si>
+    <t>Agroinsumos</t>
+  </si>
+  <si>
+    <t>Agrogan Oriente</t>
+  </si>
+  <si>
+    <t>J-12952072-3</t>
+  </si>
+  <si>
+    <t>Café</t>
+  </si>
+  <si>
+    <t>sacos</t>
+  </si>
+  <si>
+    <t>Ninguna</t>
+  </si>
+  <si>
+    <t>Javier</t>
+  </si>
+  <si>
+    <t>Sin novedad</t>
   </si>
   <si>
     <t>No</t>
   </si>
   <si>
-    <t>21/03/2025</t>
-  </si>
-  <si>
-    <t>Se ve raro</t>
-  </si>
-  <si>
-    <t>nombre2</t>
-  </si>
-  <si>
-    <t>nosealv</t>
-  </si>
-  <si>
-    <t>03/04/2025</t>
-  </si>
-  <si>
-    <t>19/04/2025</t>
-  </si>
-  <si>
-    <t>kg</t>
-  </si>
-  <si>
-    <t>11/04/2025</t>
-  </si>
-  <si>
-    <t>adasdasda</t>
-  </si>
-  <si>
-    <t>10/04/2025</t>
-  </si>
-  <si>
-    <t>26/04/2025</t>
-  </si>
-  <si>
-    <t>estado2</t>
-  </si>
-  <si>
-    <t>municipio2</t>
-  </si>
-  <si>
-    <t>parroquia2</t>
-  </si>
-  <si>
-    <t>sector2</t>
-  </si>
-  <si>
-    <t>J-20000002-2</t>
-  </si>
-  <si>
-    <t>Yuca</t>
-  </si>
-  <si>
-    <t>nombre_responsable2</t>
-  </si>
-  <si>
-    <t>02/05/2025</t>
+    <t>19/09/2025</t>
+  </si>
+  <si>
+    <t>Laura</t>
   </si>
 </sst>
 </file>
@@ -1291,34 +1240,34 @@
     </row>
     <row r="7" spans="1:67" customHeight="1" ht="33">
       <c r="A7" s="16">
-        <v>1</v>
-      </c>
-      <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2">
+        <v>4024</v>
+      </c>
+      <c r="C7" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="D7" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="E7" s="19">
+        <v>6</v>
+      </c>
+      <c r="F7" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="19">
-        <v>32</v>
-      </c>
-      <c r="F7" s="19" t="s">
+      <c r="G7" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="H7" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="I7" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="20" t="s">
+      <c r="J7" s="20" t="s">
         <v>39</v>
-      </c>
-      <c r="J7" s="20" t="s">
-        <v>40</v>
       </c>
       <c r="K7" s="20" t="s">
         <v>40</v>
@@ -1330,16 +1279,16 @@
         <v>42</v>
       </c>
       <c r="N7" s="28">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="O7" s="20" t="s">
         <v>43</v>
       </c>
       <c r="P7" s="64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q7" s="30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R7" s="30" t="s">
         <v>44</v>
@@ -1348,10 +1297,10 @@
         <v>45</v>
       </c>
       <c r="T7" s="66">
-        <v>10000001</v>
+        <v>23004072</v>
       </c>
       <c r="U7" s="65">
-        <v>10000000001</v>
+        <v>4149798833</v>
       </c>
       <c r="V7" s="65" t="s">
         <v>46</v>
@@ -1363,180 +1312,72 @@
         <v>48</v>
       </c>
       <c r="Y7" s="67" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z7" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="Z7" s="65" t="s">
-        <v>50</v>
-      </c>
       <c r="AA7" s="68">
-        <v>20000000002</v>
+        <v>4149949828</v>
       </c>
     </row>
     <row r="8" spans="1:67" customHeight="1" ht="33">
-      <c r="A8" s="16">
-        <v>2</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" s="8">
-        <v>4</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="M8" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="N8" s="8">
-        <v>5</v>
-      </c>
-      <c r="O8" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="P8" s="62">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="62">
-        <v>2</v>
-      </c>
-      <c r="R8" s="70" t="s">
-        <v>44</v>
-      </c>
-      <c r="S8" s="62" t="s">
-        <v>45</v>
-      </c>
-      <c r="T8" s="62">
-        <v>10000001</v>
-      </c>
-      <c r="U8" s="62">
-        <v>10000000001</v>
-      </c>
-      <c r="V8" s="62" t="s">
-        <v>46</v>
-      </c>
-      <c r="W8" s="62" t="s">
-        <v>47</v>
-      </c>
-      <c r="X8" s="63" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y8" s="62" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z8" s="62" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA8" s="62">
-        <v>20000000002</v>
-      </c>
+      <c r="A8" s="16"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="62"/>
+      <c r="Q8" s="62"/>
+      <c r="R8" s="70"/>
+      <c r="S8" s="62"/>
+      <c r="T8" s="62"/>
+      <c r="U8" s="62"/>
+      <c r="V8" s="62"/>
+      <c r="W8" s="62"/>
+      <c r="X8" s="63"/>
+      <c r="Y8" s="62"/>
+      <c r="Z8" s="62"/>
+      <c r="AA8" s="62"/>
     </row>
     <row r="9" spans="1:67" customHeight="1" ht="33">
-      <c r="A9" s="16">
-        <v>3</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="8">
-        <v>3</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="N9" s="8">
-        <v>5</v>
-      </c>
-      <c r="O9" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="P9" s="62">
-        <v>2</v>
-      </c>
-      <c r="Q9" s="62">
-        <v>1</v>
-      </c>
-      <c r="R9" s="70" t="s">
-        <v>44</v>
-      </c>
-      <c r="S9" s="62" t="s">
-        <v>65</v>
-      </c>
-      <c r="T9" s="62">
-        <v>20000002</v>
-      </c>
-      <c r="U9" s="62">
-        <v>20000000002</v>
-      </c>
-      <c r="V9" s="62" t="s">
-        <v>46</v>
-      </c>
-      <c r="W9" s="62" t="s">
-        <v>47</v>
-      </c>
-      <c r="X9" s="63" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y9" s="62" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z9" s="62" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA9" s="62">
-        <v>20000000002</v>
-      </c>
+      <c r="A9" s="16"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="62"/>
+      <c r="Q9" s="62"/>
+      <c r="R9" s="70"/>
+      <c r="S9" s="62"/>
+      <c r="T9" s="62"/>
+      <c r="U9" s="62"/>
+      <c r="V9" s="62"/>
+      <c r="W9" s="62"/>
+      <c r="X9" s="63"/>
+      <c r="Y9" s="62"/>
+      <c r="Z9" s="62"/>
+      <c r="AA9" s="62"/>
     </row>
     <row r="10" spans="1:67" customHeight="1" ht="33" s="7" customFormat="1">
       <c r="A10" s="16"/>

</xml_diff>